<commit_message>
day15 and day14 part 1s only
</commit_message>
<xml_diff>
--- a/visualizations/Day8_Rules.xlsx
+++ b/visualizations/Day8_Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danth\rust\aoc2021\visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462C356C-199C-4E24-A72A-FE077EBFD43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC1C2E4-ABA5-43AA-819C-9028ABAD50F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="0" windowWidth="16995" windowHeight="13800" xr2:uid="{E9FED008-D5D3-4AC6-BB85-847B971365E8}"/>
+    <workbookView xWindow="4845" yWindow="2715" windowWidth="16995" windowHeight="13800" xr2:uid="{E9FED008-D5D3-4AC6-BB85-847B971365E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
   <si>
     <t>x</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>F = CF-C</t>
+  </si>
+  <si>
+    <t>G = Size7-A-B-ECD-F</t>
   </si>
 </sst>
 </file>
@@ -215,12 +218,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -540,7 +543,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,21 +551,21 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="8" width="5.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="5" customWidth="1"/>
     <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -625,13 +628,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f>7-COUNTBLANK(B3:H3)</f>
+        <f t="shared" ref="I3:I12" si="0">7-COUNTBLANK(B3:H3)</f>
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="M3" t="s">
@@ -648,14 +651,14 @@
       <c r="G4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="7">
-        <f>7-COUNTBLANK(B4:H4)</f>
+      <c r="I4" s="6">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M4" t="s">
@@ -682,13 +685,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <f>7-COUNTBLANK(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M5" t="s">
@@ -715,13 +718,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <f>7-COUNTBLANK(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="M6" t="s">
@@ -744,14 +747,14 @@
       <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="7">
-        <f>7-COUNTBLANK(B7:H7)</f>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="M7" t="s">
@@ -778,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <f>7-COUNTBLANK(B8:H8)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="M8" t="s">
@@ -814,13 +817,13 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f>7-COUNTBLANK(B9:H9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="M9" t="s">
@@ -840,14 +843,14 @@
       <c r="G10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="7">
-        <f>7-COUNTBLANK(B10:H10)</f>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="M10" t="s">
@@ -879,11 +882,11 @@
       <c r="H11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="7">
-        <f>7-COUNTBLANK(B11:H11)</f>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M11" t="s">
@@ -913,30 +916,33 @@
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <f>7-COUNTBLANK(B12:H12)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
       <c r="J16" s="1"/>
-      <c r="L16" s="6"/>
+      <c r="L16" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K12">

</xml_diff>